<commit_message>
Update report sheets; fix bugs
</commit_message>
<xml_diff>
--- a/report/Debug/report_sheet_english.xlsx
+++ b/report/Debug/report_sheet_english.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7965" yWindow="-120" windowWidth="10815" windowHeight="7995" tabRatio="864" firstSheet="1" activeTab="10"/>
+    <workbookView xWindow="7965" yWindow="-120" windowWidth="10815" windowHeight="7995" tabRatio="864" firstSheet="19" activeTab="26"/>
   </bookViews>
   <sheets>
     <sheet name="CONTROLS" sheetId="4" r:id="rId1"/>
@@ -52,7 +52,7 @@
   <definedNames>
     <definedName name="DATE">CONTROLS!$B$1</definedName>
     <definedName name="DAY">CONTROLS!$D$5</definedName>
-    <definedName name="english_data_1" localSheetId="34">DATA_BY_COMP!$A$1:$G$83</definedName>
+    <definedName name="english_data_1" localSheetId="34">DATA_BY_COMP!$A$1:$G$84</definedName>
     <definedName name="english_data_by_unit" localSheetId="35">DATA_BY_UNIT!$A$1:$G$34</definedName>
     <definedName name="ENGLISH_REPORT_DAY">CONTROLS!$B$2</definedName>
     <definedName name="ENGLISH_WEEKLY_REPORT_DAY">CONTROLS!$B$2</definedName>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1681" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1685" uniqueCount="487">
   <si>
     <t>YEAR</t>
   </si>
@@ -1234,9 +1234,6 @@
     <t>2016:2:1:3:ZHONGHE_2_S</t>
   </si>
   <si>
-    <t xml:space="preserve"> advanced</t>
-  </si>
-  <si>
     <t>2016:2:1:3:ZHONGLI_2_E</t>
   </si>
   <si>
@@ -1568,6 +1565,12 @@
   </si>
   <si>
     <t>Tong</t>
+  </si>
+  <si>
+    <t>2016:2:1:3:SONGSHAN_E</t>
+  </si>
+  <si>
+    <t>+886963938192</t>
   </si>
 </sst>
 </file>
@@ -2890,8 +2893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5073,7 +5076,7 @@
       </c>
       <c r="D7" s="3">
         <f>MATCH($C7,DATA_BY_COMP!$A:$A,0)</f>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E7" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D7,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -5534,7 +5537,7 @@
       </c>
       <c r="D5" s="3">
         <f>MATCH($C5,DATA_BY_COMP!$A:$A,0)</f>
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E5" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D5,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -5608,7 +5611,7 @@
       </c>
       <c r="D7" s="3">
         <f>MATCH($C7,DATA_BY_COMP!$A:$A,0)</f>
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E7" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D7,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -5676,7 +5679,7 @@
       </c>
       <c r="D9" s="3">
         <f>MATCH($C9,DATA_BY_COMP!$A:$A,0)</f>
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E9" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D9,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -5744,7 +5747,7 @@
       </c>
       <c r="D11" s="3">
         <f>MATCH($C11,DATA_BY_COMP!$A:$A,0)</f>
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E11" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D11,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -6135,29 +6138,29 @@
         <f t="shared" ref="C5:C7" si="0">CONCATENATE(YEAR,":",MONTH,":",WEEK,":",DAY,":",$A5)</f>
         <v>2016:2:1:3:SONGSHAN_E</v>
       </c>
-      <c r="D5" s="3" t="e">
+      <c r="D5" s="3">
         <f>MATCH($C5,DATA_BY_COMP!$A:$A,0)</f>
-        <v>#N/A</v>
+        <v>38</v>
       </c>
       <c r="E5" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D5,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
-        <v/>
+        <v>advanced</v>
       </c>
       <c r="F5" s="15" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D5,MATCH(F$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
-        <v/>
-      </c>
-      <c r="G5" s="15" t="str">
+        <v>beginner</v>
+      </c>
+      <c r="G5" s="15">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D5,MATCH(G$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
-        <v/>
-      </c>
-      <c r="H5" s="15" t="str">
+        <v>11</v>
+      </c>
+      <c r="H5" s="15">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D5,MATCH(H$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
-        <v/>
-      </c>
-      <c r="I5" s="15" t="str">
+        <v>9</v>
+      </c>
+      <c r="I5" s="15">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D5,MATCH(I$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="K5" s="15" t="s">
         <v>163</v>
@@ -6211,7 +6214,7 @@
       </c>
       <c r="D7" s="3">
         <f>MATCH($C7,DATA_BY_COMP!$A:$A,0)</f>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E7" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D7,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -6678,7 +6681,7 @@
       </c>
       <c r="D7" s="3">
         <f>MATCH($C7,DATA_BY_COMP!$A:$A,0)</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E7" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D7,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -6826,7 +6829,7 @@
       </c>
       <c r="D11" s="3">
         <f>MATCH($C11,DATA_BY_COMP!$A:$A,0)</f>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E11" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D11,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -6900,7 +6903,7 @@
       </c>
       <c r="D13" s="3">
         <f>MATCH($C13,DATA_BY_COMP!$A:$A,0)</f>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E13" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D13,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -7297,7 +7300,7 @@
       </c>
       <c r="D5" s="3">
         <f>MATCH($C5,DATA_BY_COMP!$A:$A,0)</f>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E5" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D5,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -7519,7 +7522,7 @@
       </c>
       <c r="D11" s="3">
         <f>MATCH($C11,DATA_BY_COMP!$A:$A,0)</f>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E11" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D11,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -12812,6 +12815,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="O1:O8"/>
+    <mergeCell ref="P1:P8"/>
+    <mergeCell ref="Q1:Q8"/>
+    <mergeCell ref="R1:R8"/>
+    <mergeCell ref="S1:S8"/>
     <mergeCell ref="M1:M8"/>
     <mergeCell ref="N1:N8"/>
     <mergeCell ref="B3:B5"/>
@@ -12819,11 +12827,6 @@
     <mergeCell ref="J1:J8"/>
     <mergeCell ref="K1:K8"/>
     <mergeCell ref="L1:L8"/>
-    <mergeCell ref="O1:O8"/>
-    <mergeCell ref="P1:P8"/>
-    <mergeCell ref="Q1:Q8"/>
-    <mergeCell ref="R1:R8"/>
-    <mergeCell ref="S1:S8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -12939,7 +12942,7 @@
       </c>
       <c r="D5" s="3">
         <f>MATCH($C5,DATA_BY_COMP!$A:$A,0)</f>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E5" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D5,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -13013,7 +13016,7 @@
       </c>
       <c r="D7" s="3">
         <f>MATCH($C7,DATA_BY_COMP!$A:$A,0)</f>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E7" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D7,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -13087,7 +13090,7 @@
       </c>
       <c r="D9" s="3">
         <f>MATCH($C9,DATA_BY_COMP!$A:$A,0)</f>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E9" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D9,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -13161,7 +13164,7 @@
       </c>
       <c r="D11" s="3">
         <f>MATCH($C11,DATA_BY_COMP!$A:$A,0)</f>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E11" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D11,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -13560,7 +13563,7 @@
       </c>
       <c r="D5" s="3">
         <f>MATCH($C5,DATA_BY_COMP!$A:$A,0)</f>
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E5" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D5,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -13959,7 +13962,7 @@
       </c>
       <c r="D5" s="3">
         <f>MATCH($C5,DATA_BY_COMP!$A:$A,0)</f>
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E5" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D5,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -14033,7 +14036,7 @@
       </c>
       <c r="D7" s="3">
         <f>MATCH($C7,DATA_BY_COMP!$A:$A,0)</f>
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E7" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D7,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -14107,7 +14110,7 @@
       </c>
       <c r="D9" s="3">
         <f>MATCH($C9,DATA_BY_COMP!$A:$A,0)</f>
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E9" s="3">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D9,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -14581,7 +14584,7 @@
       </c>
       <c r="D7" s="3">
         <f>MATCH($C7,DATA_BY_COMP!$A:$A,0)</f>
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E7" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D7,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -14649,11 +14652,11 @@
       </c>
       <c r="D9" s="3">
         <f>MATCH($C9,DATA_BY_COMP!$A:$A,0)</f>
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E9" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D9,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
-        <v xml:space="preserve"> advanced</v>
+        <v>advanced</v>
       </c>
       <c r="F9" s="15">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D9,MATCH(F$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -15110,7 +15113,7 @@
       </c>
       <c r="D5" s="3">
         <f>MATCH($C5,DATA_BY_COMP!$A:$A,0)</f>
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E5" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D5,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -15184,7 +15187,7 @@
       </c>
       <c r="D7" s="3">
         <f>MATCH($C7,DATA_BY_COMP!$A:$A,0)</f>
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E7" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D7,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -15855,7 +15858,7 @@
       </c>
       <c r="D9" s="3">
         <f>MATCH($C9,DATA_BY_COMP!$A:$A,0)</f>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E9" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D9,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -15923,7 +15926,7 @@
       </c>
       <c r="D11" s="3">
         <f>MATCH($C11,DATA_BY_COMP!$A:$A,0)</f>
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E11" s="3">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D11,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -16212,7 +16215,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16316,7 +16319,7 @@
       </c>
       <c r="D5" s="3">
         <f>MATCH($C5,DATA_BY_COMP!$A:$A,0)</f>
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E5" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D5,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -16390,7 +16393,7 @@
       </c>
       <c r="D7" s="3">
         <f>MATCH($C7,DATA_BY_COMP!$A:$A,0)</f>
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E7" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D7,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -16526,7 +16529,7 @@
       </c>
       <c r="D11" s="3">
         <f>MATCH($C11,DATA_BY_COMP!$A:$A,0)</f>
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E11" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D11,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -16814,7 +16817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
@@ -17386,7 +17389,7 @@
       </c>
       <c r="D5" s="3">
         <f>MATCH($C5,DATA_BY_COMP!$A:$A,0)</f>
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E5" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D5,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -17460,7 +17463,7 @@
       </c>
       <c r="D7" s="3">
         <f>MATCH($C7,DATA_BY_COMP!$A:$A,0)</f>
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E7" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D7,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -17528,7 +17531,7 @@
       </c>
       <c r="D9" s="3">
         <f>MATCH($C9,DATA_BY_COMP!$A:$A,0)</f>
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E9" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D9,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -17921,7 +17924,7 @@
       </c>
       <c r="D5" s="3">
         <f>MATCH($C5,DATA_BY_COMP!$A:$A,0)</f>
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E5" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D5,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -17995,7 +17998,7 @@
       </c>
       <c r="D7" s="3">
         <f>MATCH($C7,DATA_BY_COMP!$A:$A,0)</f>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E7" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D7,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -18959,7 +18962,7 @@
       </c>
       <c r="D5" s="3">
         <f>MATCH($C5,DATA_BY_COMP!$A:$A,0)</f>
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E5" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D5,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -19033,7 +19036,7 @@
       </c>
       <c r="D7" s="3">
         <f>MATCH($C7,DATA_BY_COMP!$A:$A,0)</f>
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E7" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D7,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -19426,7 +19429,7 @@
       </c>
       <c r="D5" s="3">
         <f>MATCH($C5,DATA_BY_COMP!$A:$A,0)</f>
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E5" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D5,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -19568,7 +19571,7 @@
       </c>
       <c r="D9" s="3">
         <f>MATCH($C9,DATA_BY_COMP!$A:$A,0)</f>
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E9" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D9,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -20035,7 +20038,7 @@
       </c>
       <c r="D7" s="3">
         <f>MATCH($C7,DATA_BY_COMP!$A:$A,0)</f>
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E7" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D7,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -20103,7 +20106,7 @@
       </c>
       <c r="D9" s="3">
         <f>MATCH($C9,DATA_BY_COMP!$A:$A,0)</f>
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E9" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D9,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -20564,7 +20567,7 @@
       </c>
       <c r="D5" s="3">
         <f>MATCH($C5,DATA_BY_COMP!$A:$A,0)</f>
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E5" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D5,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -20638,7 +20641,7 @@
       </c>
       <c r="D7" s="3">
         <f>MATCH($C7,DATA_BY_COMP!$A:$A,0)</f>
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E7" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D7,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -21031,7 +21034,7 @@
       </c>
       <c r="D5" s="3">
         <f>MATCH($C5,DATA_BY_COMP!$A:$A,0)</f>
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E5" s="3">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D5,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -21105,7 +21108,7 @@
       </c>
       <c r="D7" s="3">
         <f>MATCH($C7,DATA_BY_COMP!$A:$A,0)</f>
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E7" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D7,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -21173,7 +21176,7 @@
       </c>
       <c r="D9" s="3">
         <f>MATCH($C9,DATA_BY_COMP!$A:$A,0)</f>
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E9" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D9,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -21241,7 +21244,7 @@
       </c>
       <c r="D11" s="3">
         <f>MATCH($C11,DATA_BY_COMP!$A:$A,0)</f>
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E11" s="3">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D11,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -21527,10 +21530,10 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G83"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H77" sqref="H77"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21567,10 +21570,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>462</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>463</v>
       </c>
       <c r="C2" s="32">
         <v>0</v>
@@ -21590,13 +21593,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D3" s="32">
         <v>3</v>
@@ -21613,7 +21616,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>65</v>
@@ -21682,7 +21685,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>68</v>
@@ -21705,13 +21708,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>69</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D8" s="32">
         <v>4</v>
@@ -21751,7 +21754,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>71</v>
@@ -21760,7 +21763,7 @@
         <v>358</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E10" s="32">
         <v>8</v>
@@ -21774,7 +21777,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>72</v>
@@ -21797,7 +21800,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>73</v>
@@ -21981,7 +21984,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>132</v>
@@ -22004,7 +22007,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>79</v>
@@ -22027,13 +22030,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="32" t="s">
         <v>391</v>
-      </c>
-      <c r="C22" s="32" t="s">
-        <v>392</v>
       </c>
       <c r="D22" s="32">
         <v>6</v>
@@ -22050,7 +22053,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>80</v>
@@ -22059,7 +22062,7 @@
         <v>348</v>
       </c>
       <c r="D23" s="32" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E23" s="32" t="s">
         <v>358</v>
@@ -22096,7 +22099,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>82</v>
@@ -22142,13 +22145,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C27" s="32" t="s">
         <v>434</v>
-      </c>
-      <c r="C27" s="32" t="s">
-        <v>435</v>
       </c>
       <c r="D27" s="32">
         <v>3</v>
@@ -22165,7 +22168,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>84</v>
@@ -22188,7 +22191,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>85</v>
@@ -22234,13 +22237,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="32" t="s">
         <v>466</v>
-      </c>
-      <c r="C31" s="32" t="s">
-        <v>467</v>
       </c>
       <c r="D31" s="32">
         <v>7</v>
@@ -22257,7 +22260,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>86</v>
@@ -22280,7 +22283,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>136</v>
@@ -22349,7 +22352,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>89</v>
@@ -22395,22 +22398,22 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>400</v>
+        <v>485</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>91</v>
+        <v>486</v>
       </c>
       <c r="C38" s="32" t="s">
-        <v>442</v>
-      </c>
-      <c r="D38" s="32">
-        <v>15</v>
+        <v>333</v>
+      </c>
+      <c r="D38" s="32" t="s">
+        <v>348</v>
       </c>
       <c r="E38" s="32">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F38" s="32">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G38" s="32">
         <v>2</v>
@@ -22418,45 +22421,45 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C39" s="32" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="D39" s="32">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E39" s="32">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F39" s="32">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G39" s="32">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C40" s="32" t="s">
-        <v>333</v>
+        <v>443</v>
       </c>
       <c r="D40" s="32">
         <v>7</v>
       </c>
       <c r="E40" s="32">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F40" s="32">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G40" s="32">
         <v>1</v>
@@ -22464,45 +22467,45 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C41" s="32" t="s">
-        <v>358</v>
+        <v>333</v>
       </c>
       <c r="D41" s="32">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E41" s="32">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F41" s="32">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G41" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>352</v>
+        <v>402</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C42" s="32" t="s">
-        <v>333</v>
+        <v>358</v>
       </c>
       <c r="D42" s="32">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E42" s="32">
         <v>8</v>
       </c>
       <c r="F42" s="32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G42" s="32">
         <v>0</v>
@@ -22510,19 +22513,19 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>404</v>
+        <v>352</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C43" s="32" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="D43" s="32">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E43" s="32">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F43" s="32">
         <v>0</v>
@@ -22533,22 +22536,22 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>353</v>
+        <v>403</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="C44" s="32" t="s">
-        <v>333</v>
+        <v>348</v>
       </c>
       <c r="D44" s="32">
         <v>6</v>
       </c>
       <c r="E44" s="32">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F44" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G44" s="32">
         <v>0</v>
@@ -22556,22 +22559,22 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>130</v>
+        <v>83</v>
       </c>
       <c r="C45" s="32" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D45" s="32">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E45" s="32">
+        <v>6</v>
+      </c>
+      <c r="F45" s="32">
         <v>1</v>
-      </c>
-      <c r="F45" s="32">
-        <v>0</v>
       </c>
       <c r="G45" s="32">
         <v>0</v>
@@ -22579,42 +22582,42 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>405</v>
+        <v>354</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>97</v>
+        <v>130</v>
       </c>
       <c r="C46" s="32" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="D46" s="32">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E46" s="32">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F46" s="32">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G46" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>468</v>
+        <v>404</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>469</v>
+        <v>97</v>
       </c>
       <c r="C47" s="32" t="s">
-        <v>155</v>
+        <v>348</v>
       </c>
       <c r="D47" s="32">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E47" s="32">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F47" s="32">
         <v>4</v>
@@ -22625,111 +22628,111 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C48" s="32" t="s">
-        <v>472</v>
-      </c>
-      <c r="D48" s="32" t="s">
-        <v>358</v>
+        <v>155</v>
+      </c>
+      <c r="D48" s="32">
+        <v>13</v>
       </c>
       <c r="E48" s="32">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F48" s="32">
         <v>4</v>
       </c>
       <c r="G48" s="32">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>355</v>
+        <v>469</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>98</v>
+        <v>470</v>
       </c>
       <c r="C49" s="32" t="s">
-        <v>356</v>
-      </c>
-      <c r="D49" s="32">
-        <v>3</v>
+        <v>471</v>
+      </c>
+      <c r="D49" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="E49" s="32">
+        <v>5</v>
+      </c>
+      <c r="F49" s="32">
+        <v>4</v>
+      </c>
+      <c r="G49" s="32">
         <v>2</v>
-      </c>
-      <c r="F49" s="32">
-        <v>0</v>
-      </c>
-      <c r="G49" s="32">
-        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C50" s="32" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D50" s="32">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E50" s="32">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F50" s="32">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G50" s="32">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="C51" s="32">
-        <v>0</v>
+        <v>99</v>
+      </c>
+      <c r="C51" s="32" t="s">
+        <v>358</v>
       </c>
       <c r="D51" s="32">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E51" s="32">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F51" s="32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G51" s="32">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>406</v>
+        <v>359</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C52" s="32" t="s">
-        <v>152</v>
+        <v>360</v>
+      </c>
+      <c r="C52" s="32">
+        <v>0</v>
       </c>
       <c r="D52" s="32">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E52" s="32">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F52" s="32">
         <v>0</v>
@@ -22740,22 +22743,22 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>100</v>
+        <v>131</v>
       </c>
       <c r="C53" s="32" t="s">
-        <v>374</v>
+        <v>152</v>
       </c>
       <c r="D53" s="32">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E53" s="32">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="F53" s="32">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G53" s="32">
         <v>0</v>
@@ -22763,22 +22766,22 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>361</v>
+        <v>406</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C54" s="32" t="s">
-        <v>358</v>
+        <v>333</v>
       </c>
       <c r="D54" s="32">
         <v>11</v>
       </c>
       <c r="E54" s="32">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F54" s="32">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G54" s="32">
         <v>0</v>
@@ -22786,22 +22789,22 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>408</v>
+        <v>361</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C55" s="32" t="s">
-        <v>461</v>
-      </c>
-      <c r="D55" s="32" t="s">
-        <v>356</v>
+        <v>358</v>
+      </c>
+      <c r="D55" s="32">
+        <v>11</v>
       </c>
       <c r="E55" s="32">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F55" s="32">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G55" s="32">
         <v>0</v>
@@ -22809,22 +22812,22 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>362</v>
+        <v>407</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C56" s="32">
-        <v>0</v>
-      </c>
-      <c r="D56" s="32">
-        <v>0</v>
+        <v>102</v>
+      </c>
+      <c r="C56" s="32" t="s">
+        <v>460</v>
+      </c>
+      <c r="D56" s="32" t="s">
+        <v>356</v>
       </c>
       <c r="E56" s="32">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F56" s="32">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G56" s="32">
         <v>0</v>
@@ -22832,22 +22835,22 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C57" s="32" t="s">
-        <v>358</v>
+        <v>103</v>
+      </c>
+      <c r="C57" s="32">
+        <v>0</v>
       </c>
       <c r="D57" s="32">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E57" s="32">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F57" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G57" s="32">
         <v>0</v>
@@ -22855,22 +22858,22 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>409</v>
+        <v>363</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C58" s="32" t="s">
-        <v>152</v>
+        <v>358</v>
       </c>
       <c r="D58" s="32">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E58" s="32">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F58" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G58" s="32">
         <v>0</v>
@@ -22878,19 +22881,19 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C59" s="32">
-        <v>0</v>
+        <v>105</v>
+      </c>
+      <c r="C59" s="32" t="s">
+        <v>152</v>
       </c>
       <c r="D59" s="32">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E59" s="32">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F59" s="32">
         <v>0</v>
@@ -22901,19 +22904,19 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>364</v>
+        <v>409</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C60" s="32" t="s">
-        <v>152</v>
+        <v>106</v>
+      </c>
+      <c r="C60" s="32">
+        <v>0</v>
       </c>
       <c r="D60" s="32">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E60" s="32">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F60" s="32">
         <v>0</v>
@@ -22924,16 +22927,16 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C61" s="32" t="s">
-        <v>358</v>
+        <v>152</v>
       </c>
       <c r="D61" s="32">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E61" s="32">
         <v>4</v>
@@ -22947,16 +22950,16 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>411</v>
+        <v>365</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C62" s="32" t="s">
-        <v>152</v>
+        <v>358</v>
       </c>
       <c r="D62" s="32">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E62" s="32">
         <v>4</v>
@@ -22970,68 +22973,68 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C63" s="32" t="s">
-        <v>473</v>
-      </c>
-      <c r="D63" s="32" t="s">
-        <v>474</v>
-      </c>
-      <c r="E63" s="32" t="s">
-        <v>475</v>
+        <v>152</v>
+      </c>
+      <c r="D63" s="32">
+        <v>7</v>
+      </c>
+      <c r="E63" s="32">
+        <v>4</v>
       </c>
       <c r="F63" s="32">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G63" s="32">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>332</v>
+        <v>411</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C64" s="32" t="s">
-        <v>358</v>
-      </c>
-      <c r="D64" s="32">
-        <v>5</v>
-      </c>
-      <c r="E64" s="32">
-        <v>1</v>
+        <v>472</v>
+      </c>
+      <c r="D64" s="32" t="s">
+        <v>473</v>
+      </c>
+      <c r="E64" s="32" t="s">
+        <v>474</v>
       </c>
       <c r="F64" s="32">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G64" s="32">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C65" s="32" t="s">
-        <v>335</v>
+        <v>358</v>
       </c>
       <c r="D65" s="32">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E65" s="32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G65" s="32">
         <v>0</v>
@@ -23039,22 +23042,22 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>366</v>
+        <v>334</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C66" s="32" t="s">
-        <v>367</v>
+        <v>335</v>
       </c>
       <c r="D66" s="32">
         <v>3</v>
       </c>
       <c r="E66" s="32">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F66" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G66" s="32">
         <v>0</v>
@@ -23062,22 +23065,22 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>476</v>
+        <v>366</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>477</v>
+        <v>113</v>
       </c>
       <c r="C67" s="32" t="s">
-        <v>478</v>
+        <v>367</v>
       </c>
       <c r="D67" s="32">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E67" s="32">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F67" s="32">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G67" s="32">
         <v>0</v>
@@ -23085,22 +23088,22 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>413</v>
+        <v>475</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>114</v>
+        <v>476</v>
       </c>
       <c r="C68" s="32" t="s">
-        <v>339</v>
+        <v>477</v>
       </c>
       <c r="D68" s="32">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E68" s="32">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F68" s="32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G68" s="32">
         <v>0</v>
@@ -23108,19 +23111,19 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>368</v>
+        <v>412</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C69" s="32" t="s">
-        <v>369</v>
+        <v>339</v>
       </c>
       <c r="D69" s="32">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E69" s="32">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F69" s="32">
         <v>0</v>
@@ -23131,19 +23134,19 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C70" s="32" t="s">
-        <v>152</v>
+        <v>369</v>
       </c>
       <c r="D70" s="32">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E70" s="32">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F70" s="32">
         <v>0</v>
@@ -23154,68 +23157,68 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>414</v>
+        <v>370</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C71" s="32" t="s">
-        <v>479</v>
-      </c>
-      <c r="D71" s="32" t="s">
-        <v>480</v>
-      </c>
-      <c r="E71" s="32" t="s">
-        <v>392</v>
-      </c>
-      <c r="F71" s="32" t="s">
-        <v>481</v>
-      </c>
-      <c r="G71" s="32" t="s">
-        <v>482</v>
+        <v>152</v>
+      </c>
+      <c r="D71" s="32">
+        <v>3</v>
+      </c>
+      <c r="E71" s="32">
+        <v>3</v>
+      </c>
+      <c r="F71" s="32">
+        <v>0</v>
+      </c>
+      <c r="G71" s="32">
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>336</v>
+        <v>413</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C72" s="32" t="s">
-        <v>337</v>
-      </c>
-      <c r="D72" s="32">
-        <v>7</v>
-      </c>
-      <c r="E72" s="32">
-        <v>6</v>
-      </c>
-      <c r="F72" s="32">
-        <v>1</v>
-      </c>
-      <c r="G72" s="32">
-        <v>0</v>
+        <v>478</v>
+      </c>
+      <c r="D72" s="32" t="s">
+        <v>479</v>
+      </c>
+      <c r="E72" s="32" t="s">
+        <v>391</v>
+      </c>
+      <c r="F72" s="32" t="s">
+        <v>480</v>
+      </c>
+      <c r="G72" s="32" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>371</v>
+        <v>336</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C73" s="32" t="s">
-        <v>372</v>
+        <v>337</v>
       </c>
       <c r="D73" s="32">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E73" s="32">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F73" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G73" s="32">
         <v>0</v>
@@ -23223,22 +23226,22 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C74" s="32" t="s">
-        <v>333</v>
+        <v>372</v>
       </c>
       <c r="D74" s="32">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E74" s="32">
         <v>3</v>
       </c>
       <c r="F74" s="32">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G74" s="32">
         <v>0</v>
@@ -23246,22 +23249,22 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>415</v>
+        <v>373</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C75" s="32" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="D75" s="32">
         <v>4</v>
       </c>
       <c r="E75" s="32">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F75" s="32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G75" s="32">
         <v>0</v>
@@ -23269,137 +23272,137 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>375</v>
+        <v>414</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="C76" s="32" t="s">
-        <v>376</v>
+        <v>348</v>
       </c>
       <c r="D76" s="32">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E76" s="32">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F76" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G76" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>483</v>
+        <v>374</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="C77" s="32" t="s">
-        <v>358</v>
+        <v>375</v>
       </c>
       <c r="D77" s="32">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E77" s="32">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F77" s="32">
         <v>0</v>
       </c>
       <c r="G77" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>416</v>
+        <v>482</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C78" s="32" t="s">
-        <v>161</v>
+        <v>358</v>
       </c>
       <c r="D78" s="32">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E78" s="32">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F78" s="32">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G78" s="32">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>377</v>
+        <v>415</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C79" s="32" t="s">
-        <v>378</v>
+        <v>161</v>
       </c>
       <c r="D79" s="32">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E79" s="32">
+        <v>10</v>
+      </c>
+      <c r="F79" s="32">
         <v>2</v>
       </c>
-      <c r="F79" s="32">
-        <v>1</v>
-      </c>
       <c r="G79" s="32">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>417</v>
+        <v>376</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C80" s="32" t="s">
-        <v>484</v>
-      </c>
-      <c r="D80" s="32" t="s">
-        <v>485</v>
+        <v>377</v>
+      </c>
+      <c r="D80" s="32">
+        <v>4</v>
       </c>
       <c r="E80" s="32">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F80" s="32">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G80" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C81" s="32">
-        <v>0</v>
-      </c>
-      <c r="D81" s="32">
-        <v>0</v>
+        <v>133</v>
+      </c>
+      <c r="C81" s="32" t="s">
+        <v>483</v>
+      </c>
+      <c r="D81" s="32" t="s">
+        <v>484</v>
       </c>
       <c r="E81" s="32">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F81" s="32">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G81" s="32">
         <v>0</v>
@@ -23407,22 +23410,22 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C82" s="32" t="s">
-        <v>420</v>
+        <v>125</v>
+      </c>
+      <c r="C82" s="32">
+        <v>0</v>
       </c>
       <c r="D82" s="32">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E82" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F82" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G82" s="32">
         <v>0</v>
@@ -23430,24 +23433,47 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="B83" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C83" s="32" t="s">
+        <v>419</v>
+      </c>
+      <c r="D83" s="32">
+        <v>5</v>
+      </c>
+      <c r="E83" s="32">
+        <v>1</v>
+      </c>
+      <c r="F83" s="32">
+        <v>1</v>
+      </c>
+      <c r="G83" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C83" s="32" t="s">
+      <c r="C84" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="D83" s="32">
-        <v>0</v>
-      </c>
-      <c r="E83" s="32">
-        <v>0</v>
-      </c>
-      <c r="F83" s="32">
-        <v>0</v>
-      </c>
-      <c r="G83" s="32">
+      <c r="D84" s="32">
+        <v>0</v>
+      </c>
+      <c r="E84" s="32">
+        <v>0</v>
+      </c>
+      <c r="F84" s="32">
+        <v>0</v>
+      </c>
+      <c r="G84" s="32">
         <v>0</v>
       </c>
     </row>
@@ -23492,13 +23518,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -23515,7 +23541,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>65</v>
@@ -23538,7 +23564,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>68</v>
@@ -23561,7 +23587,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>71</v>
@@ -23570,7 +23596,7 @@
         <v>358</v>
       </c>
       <c r="D5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E5">
         <v>8</v>
@@ -23584,7 +23610,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>73</v>
@@ -23607,7 +23633,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>76</v>
@@ -23630,7 +23656,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>78</v>
@@ -23653,7 +23679,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>80</v>
@@ -23662,7 +23688,7 @@
         <v>348</v>
       </c>
       <c r="D9" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E9" t="s">
         <v>358</v>
@@ -23676,7 +23702,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>82</v>
@@ -23699,13 +23725,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>432</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" t="s">
         <v>434</v>
-      </c>
-      <c r="C11" t="s">
-        <v>435</v>
       </c>
       <c r="D11">
         <v>6</v>
@@ -23722,7 +23748,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>63</v>
@@ -23745,13 +23771,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C13" t="s">
         <v>391</v>
-      </c>
-      <c r="C13" t="s">
-        <v>392</v>
       </c>
       <c r="D13">
         <v>20</v>
@@ -23768,7 +23794,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>136</v>
@@ -23791,7 +23817,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>88</v>
@@ -23814,7 +23840,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>115</v>
@@ -23837,13 +23863,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>91</v>
       </c>
       <c r="C17" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D17">
         <v>15</v>
@@ -23860,13 +23886,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C18" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D18">
         <v>25</v>
@@ -23883,7 +23909,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>72</v>
@@ -23906,7 +23932,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>83</v>
@@ -23929,7 +23955,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>98</v>
@@ -23952,7 +23978,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>99</v>
@@ -23975,7 +24001,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>85</v>
@@ -23998,7 +24024,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>67</v>
@@ -24021,7 +24047,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>128</v>
@@ -24044,7 +24070,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>108</v>
@@ -24067,7 +24093,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>70</v>
@@ -24090,7 +24116,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>111</v>
@@ -24113,7 +24139,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>132</v>
@@ -24136,7 +24162,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>116</v>
@@ -24159,7 +24185,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>121</v>
@@ -24182,7 +24208,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>122</v>
@@ -24205,13 +24231,13 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>124</v>
       </c>
       <c r="C33" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D33">
         <v>4</v>
@@ -24228,13 +24254,13 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C34" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D34" t="s">
         <v>356</v>
@@ -24259,7 +24285,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25365,7 +25391,7 @@
       </c>
       <c r="D5" s="3">
         <f>MATCH($C5,DATA_BY_COMP!$A:$A,0)</f>
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E5" s="3" t="str">
         <f>IFERROR(INDEX(DATA_BY_COMP!$A:$AA,$D5,MATCH(E$4,DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>

</xml_diff>